<commit_message>
GR&GE - Cap. 4
</commit_message>
<xml_diff>
--- a/Lista de exercícios - Manzano/Atividades do capítulo 5/GE & GR do capítulo/Planilha de grau Nº5.xlsx
+++ b/Lista de exercícios - Manzano/Atividades do capítulo 5/GE & GR do capítulo/Planilha de grau Nº5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justd\Documents\MeuProjetos\Códigos em Linguagem C\Lista de exercícios - Manzano\Atividades do capítulo 5\GE &amp; GR do capítulo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96575EC-3865-4EA9-BECC-D848347E30A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B06DBE-1E9B-45CE-B1CD-B19F34A47137}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7C5CAC48-2255-42A7-8E2C-4290F3FEA30D}"/>
   </bookViews>
@@ -513,7 +513,7 @@
   <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,10 +550,10 @@
         <v>4</v>
       </c>
       <c r="E3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -567,7 +567,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -577,8 +577,12 @@
       <c r="D5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="2:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -588,8 +592,12 @@
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="2:7" ht="18.75" x14ac:dyDescent="0.4">
@@ -607,8 +615,12 @@
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>3</v>
+      </c>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="2:7" ht="18.75" x14ac:dyDescent="0.4">

</xml_diff>